<commit_message>
updated 3rd _TerVer lab
</commit_message>
<xml_diff>
--- a/_TerVer/_labs/lab03/Lab03.xlsx
+++ b/_TerVer/_labs/lab03/Lab03.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20393"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48299408-B499-4989-918C-AD316CB81464}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
   </bookViews>
   <sheets>
     <sheet name="Задача №1" sheetId="3" r:id="rId1"/>
@@ -159,7 +158,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -388,6 +387,10 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -400,15 +403,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Warning Text" xfId="2" builtinId="11"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Текст предупреждения" xfId="2" builtinId="11"/>
+    <cellStyle name="Хороший" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1621,11 +1620,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1634,13 +1633,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="28" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="11"/>
@@ -1649,14 +1648,14 @@
       <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="32">
+      <c r="B2" s="28">
         <f>15.6^2</f>
         <v>243.35999999999999</v>
       </c>
-      <c r="C2" s="32">
+      <c r="C2" s="28">
         <v>16</v>
       </c>
       <c r="D2" s="11"/>
@@ -1670,14 +1669,14 @@
       <c r="G2" s="11"/>
     </row>
     <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="32">
+      <c r="B3" s="28">
         <f>9.8^2</f>
         <v>96.04000000000002</v>
       </c>
-      <c r="C3" s="32">
+      <c r="C3" s="28">
         <v>21</v>
       </c>
       <c r="D3" s="11"/>
@@ -1744,7 +1743,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2181,7 +2180,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2211,12 +2210,12 @@
       <c r="A2" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="30"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="32"/>
       <c r="F2" s="20"/>
       <c r="G2" s="7" t="s">
         <v>8</v>
@@ -2353,17 +2352,17 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
       <c r="D8" s="16"/>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
       <c r="H8" s="16"/>
       <c r="I8" s="16"/>
       <c r="J8" s="16"/>

</xml_diff>